<commit_message>
v0.92.5: All import cards installed and validated. Features: Fixed menu jumping in Database/Validation views, automatic navigation for all import types, domain field visibility in combined view, standardized record layouts.
</commit_message>
<xml_diff>
--- a/FLC/Templates/Cluster_template.xlsx
+++ b/FLC/Templates/Cluster_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mirko/Library/Mobile Documents/com~apple~CloudDocs/ONTWIKKEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5295A317-38B9-6147-A8A5-255D720A54FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC9C852-3084-174A-9544-2D2F1CEDC3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="760" windowWidth="29540" windowHeight="18880" xr2:uid="{5B1D9164-7E89-F143-8CBA-963F7DE74F5E}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Department</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Cluster Data Collection Template</t>
+  </si>
+  <si>
+    <t>Migration Cluster Readiness</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1217D71-7EC5-D346-9B14-81E7D434F202}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,10 +490,10 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -498,7 +501,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -506,7 +509,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -514,16 +517,16 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -531,7 +534,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -544,8 +547,11 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>